<commit_message>
v1.2.99.6: The big sound re-work
new XML attribute soundMaxRpm => RPM that corresponds to sound at
original maxRpm from vehicle xml
</commit_message>
<xml_diff>
--- a/Documents/hydro.xlsx
+++ b/Documents/hydro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17160" yWindow="0" windowWidth="13200" windowHeight="11520"/>
+    <workbookView xWindow="20280" yWindow="0" windowWidth="13200" windowHeight="11520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>ratio</t>
   </si>
@@ -56,9 +56,6 @@
     <t>idleSpeed1</t>
   </si>
   <si>
-    <t>idleSpeed2</t>
-  </si>
-  <si>
     <t>minSpeed</t>
   </si>
   <si>
@@ -105,6 +102,45 @@
   </si>
   <si>
     <t>rpm60</t>
+  </si>
+  <si>
+    <t>speed4</t>
+  </si>
+  <si>
+    <t>speed3</t>
+  </si>
+  <si>
+    <t>gear</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>fromSpeed</t>
+  </si>
+  <si>
+    <t>toSpeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;hydrostatic&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/hydrostatic&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;gears shiftTimeMs="-1" clutchRatio="1" defaultGear="1" reverseReset="false" automatic="true"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/gears&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;reverse ratio="1" shiftTimeMs="0" /&gt;</t>
+  </si>
+  <si>
+    <t>idleSpeed4</t>
+  </si>
+  <si>
+    <t>idleSpeed</t>
   </si>
 </sst>
 </file>
@@ -157,7 +193,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -172,6 +226,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -288,22 +348,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.208333333333333E-3</c:v>
+                  <c:v>2.0202020202020207E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.66666700000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91999999999999993</c:v>
+                  <c:v>0.90000009999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.08</c:v>
+                  <c:v>1.0999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4</c:v>
+                  <c:v>1.3333330000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -315,22 +375,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.140625</c:v>
+                  <c:v>0.11111111111111113</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.2</c:v>
+                  <c:v>3.6666685000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.839999999999996</c:v>
+                  <c:v>4.9500005499999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.160000000000004</c:v>
+                  <c:v>6.0499994500000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.799999999999997</c:v>
+                  <c:v>7.3333315000000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -342,11 +402,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$4</c:f>
+              <c:f>Sheet1!$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>speed2</c:v>
+                  <c:v>speed4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -382,49 +442,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.208333333333333E-3</c:v>
+                  <c:v>2.0202020202020207E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.66666700000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91999999999999993</c:v>
+                  <c:v>0.90000009999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.08</c:v>
+                  <c:v>1.0999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4</c:v>
+                  <c:v>1.3333330000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$10</c:f>
+              <c:f>Sheet1!$F$5:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.26041666666666663</c:v>
+                  <c:v>0.86868686868686895</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>28.666681000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>38.700004299999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>47.299995700000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70</c:v>
+                  <c:v>57.333319000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -436,7 +496,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$4</c:f>
+              <c:f>Sheet1!$G$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -476,49 +536,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.208333333333333E-3</c:v>
+                  <c:v>2.0202020202020207E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.66666700000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91999999999999993</c:v>
+                  <c:v>0.90000009999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.08</c:v>
+                  <c:v>1.0999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4</c:v>
+                  <c:v>1.3333330000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$10</c:f>
+              <c:f>Sheet1!$G$5:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="0.0000">
-                  <c:v>0.05</c:v>
+                  <c:v>5.000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.76</c:v>
+                  <c:v>1.650000825</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.831999999999999</c:v>
+                  <c:v>2.2275002474999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.6</c:v>
+                  <c:v>2.4750000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.368000000000002</c:v>
+                  <c:v>2.7224997525000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.439999999999998</c:v>
+                  <c:v>3.2999991750000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -530,11 +590,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$4</c:f>
+              <c:f>Sheet1!$H$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>idleSpeed2</c:v>
+                  <c:v>idleSpeed4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -570,49 +630,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.208333333333333E-3</c:v>
+                  <c:v>2.0202020202020207E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.66666700000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91999999999999993</c:v>
+                  <c:v>0.90000009999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.08</c:v>
+                  <c:v>1.0999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4</c:v>
+                  <c:v>1.3333330000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$5:$F$10</c:f>
+              <c:f>Sheet1!$H$5:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="0.00000">
-                  <c:v>9.2592592592592587E-2</c:v>
+                  <c:v>0.39090909090909104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.666666666666666</c:v>
+                  <c:v>12.900006450000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.355555555555554</c:v>
+                  <c:v>17.415001934999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.777777777777779</c:v>
+                  <c:v>19.350000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.2</c:v>
+                  <c:v>21.284998065000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.888888888888889</c:v>
+                  <c:v>25.799993550000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -627,8 +687,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="297578568"/>
-        <c:axId val="297581312"/>
+        <c:axId val="420084928"/>
+        <c:axId val="420090808"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -678,22 +738,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.208333333333333E-3</c:v>
+                  <c:v>2.0202020202020207E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.66666700000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91999999999999993</c:v>
+                  <c:v>0.90000009999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.08</c:v>
+                  <c:v>1.0999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4</c:v>
+                  <c:v>1.3333330000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -705,7 +765,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.7</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.88</c:v>
@@ -735,11 +795,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="297579744"/>
-        <c:axId val="297583272"/>
+        <c:axId val="420091984"/>
+        <c:axId val="420089632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="297578568"/>
+        <c:axId val="420084928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -796,12 +856,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297581312"/>
+        <c:crossAx val="420090808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297581312"/>
+        <c:axId val="420090808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -859,12 +919,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297578568"/>
+        <c:crossAx val="420084928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297583272"/>
+        <c:axId val="420089632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,12 +967,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297579744"/>
+        <c:crossAx val="420091984"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297579744"/>
+        <c:axId val="420091984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -922,7 +982,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297583272"/>
+        <c:crossAx val="420089632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1565,12 +1625,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
@@ -1595,31 +1655,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:I10" totalsRowShown="0">
-  <autoFilter ref="A4:I10"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:K10" totalsRowShown="0">
+  <autoFilter ref="A4:K10"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="ratio"/>
     <tableColumn id="2" name="factor"/>
-    <tableColumn id="3" name="speed1" dataDxfId="6">
+    <tableColumn id="3" name="speed1" dataDxfId="14">
       <calculatedColumnFormula>Table1[[#This Row],[ratio]]*Table2[s1]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="speed2" dataDxfId="5">
+    <tableColumn id="11" name="speed3" dataDxfId="13">
+      <calculatedColumnFormula>Table1[[#This Row],[ratio]]*Table2[s2]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="speed2" dataDxfId="12">
+      <calculatedColumnFormula>Table1[[#This Row],[ratio]]*Table2[s3]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="speed4" dataDxfId="11">
       <calculatedColumnFormula>Table1[[#This Row],[ratio]]*Table2[s4]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="idleSpeed1" dataDxfId="4">
+    <tableColumn id="7" name="idleSpeed1" dataDxfId="10">
       <calculatedColumnFormula>Table1[[#This Row],[speed1]]*Table2[idle]/Table2[rated]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="idleSpeed2" dataDxfId="3">
-      <calculatedColumnFormula>Table1[[#This Row],[speed2]]*Table2[idle]/Table2[rated]</calculatedColumnFormula>
+    <tableColumn id="6" name="idleSpeed4" dataDxfId="9">
+      <calculatedColumnFormula>Table1[[#This Row],[speed4]]*Table2[idle]/Table2[rated]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="ratio1" dataDxfId="2">
+    <tableColumn id="9" name="ratio1" dataDxfId="8">
       <calculatedColumnFormula>Table2[rated]/(Table1[[#This Row],[speed1]]/3.6 * 60 / (1*2*PI()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="ratio2" dataDxfId="1">
-      <calculatedColumnFormula>Table2[rated]/(Table1[[#This Row],[speed2]]/3.6 * 60 / (1*2*PI()))</calculatedColumnFormula>
+    <tableColumn id="8" name="ratio2" dataDxfId="7">
+      <calculatedColumnFormula>Table2[rated]/(Table1[[#This Row],[speed4]]/3.6 * 60 / (1*2*PI()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="xml" dataDxfId="0">
-      <calculatedColumnFormula>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt;")</calculatedColumnFormula>
+    <tableColumn id="5" name="xml" dataDxfId="6">
+      <calculatedColumnFormula>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt; &lt;!-- ",ROUND(Table1[[#This Row],[idleSpeed1]],2)," .. ",ROUND(Table1[[#This Row],[speed4]],1)," --&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1655,6 +1721,34 @@
     </tableColumn>
     <tableColumn id="17" name="rpm60">
       <calculatedColumnFormula>60/(Table2[s4]*(1+Table2[range]))*Table2[rated]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="E12:K16" totalsRowShown="0">
+  <autoFilter ref="E12:K16"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="gear"/>
+    <tableColumn id="2" name="speed" dataDxfId="5">
+      <calculatedColumnFormula>INDEX(Table2[],1,Table3[[#This Row],[gear]]+1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="minSpeed" dataDxfId="2">
+      <calculatedColumnFormula>$A$5*Table3[[#This Row],[speed]]*Table2[idle]/Table2[rated]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="idleSpeed" dataDxfId="1">
+      <calculatedColumnFormula>$A$6*Table3[[#This Row],[speed]]*Table2[idle]/Table2[rated]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="fromSpeed" dataDxfId="4">
+      <calculatedColumnFormula>$A$6*Table3[[#This Row],[speed]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="toSpeed" dataDxfId="3">
+      <calculatedColumnFormula>$A$10*Table3[[#This Row],[speed]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="xml" dataDxfId="0">
+      <calculatedColumnFormula>CONCATENATE("        &lt;gear speed=""",ROUND(Table3[[#This Row],[speed]],2),""" name=""""/&gt; &lt;!-- ",ROUND(Table3[[#This Row],[minSpeed]],2)," ",ROUND(Table3[[#This Row],[idleSpeed]],2)," ",ROUND(Table3[[#This Row],[fromSpeed]],0)," ",ROUND(Table3[[#This Row],[toSpeed]],0),"--&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1924,10 +2018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L4" sqref="L4:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,26 +2030,26 @@
     <col min="5" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" customWidth="1"/>
     <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -1964,37 +2058,37 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
         <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -2002,32 +2096,32 @@
         <v>0.05</v>
       </c>
       <c r="B2">
-        <v>27</v>
+        <v>5.5</v>
       </c>
       <c r="C2">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F2">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="G2">
-        <v>2250</v>
+        <v>2000</v>
       </c>
       <c r="H2">
         <f>Table2[minSpeed]/Table2[s1]/Table2[idle]*Table2[rated]</f>
-        <v>5.208333333333333E-3</v>
+        <v>2.0202020202020207E-2</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.4</v>
+        <v>0.33333299999999999</v>
       </c>
       <c r="K2">
         <v>0.88</v>
@@ -2036,25 +2130,25 @@
         <v>0.98</v>
       </c>
       <c r="M2">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="N2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="O2">
         <v>0.8</v>
       </c>
       <c r="P2">
         <f>40/(Table2[s4]*(1+Table2[range]))*Table2[rated]</f>
-        <v>1285.7142857142856</v>
+        <v>1395.3491860465988</v>
       </c>
       <c r="Q2">
         <f>50/(Table2[s4]*(1+Table2[range]))*Table2[rated]</f>
-        <v>1607.1428571428571</v>
+        <v>1744.1864825582484</v>
       </c>
       <c r="R2">
         <f>60/(Table2[s4]*(1+Table2[range]))*Table2[rated]</f>
-        <v>1928.5714285714284</v>
+        <v>2093.023779069898</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2068,66 +2162,87 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>Table2[minRatio]</f>
-        <v>5.208333333333333E-3</v>
+        <v>2.0202020202020207E-2</v>
       </c>
       <c r="B5">
         <f>Table2[zeroEff]</f>
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="C5">
         <f>Table1[[#This Row],[ratio]]*Table2[s1]</f>
-        <v>0.140625</v>
+        <v>0.11111111111111113</v>
       </c>
       <c r="D5">
+        <f>Table1[[#This Row],[ratio]]*Table2[s2]</f>
+        <v>0.22222222222222227</v>
+      </c>
+      <c r="E5">
+        <f>Table1[[#This Row],[ratio]]*Table2[s3]</f>
+        <v>0.44444444444444453</v>
+      </c>
+      <c r="F5">
         <f>Table1[[#This Row],[ratio]]*Table2[s4]</f>
-        <v>0.26041666666666663</v>
-      </c>
-      <c r="E5" s="3">
+        <v>0.86868686868686895</v>
+      </c>
+      <c r="G5" s="3">
         <f>Table1[[#This Row],[speed1]]*Table2[idle]/Table2[rated]</f>
-        <v>0.05</v>
-      </c>
-      <c r="F5" s="4">
-        <f>Table1[[#This Row],[speed2]]*Table2[idle]/Table2[rated]</f>
-        <v>9.2592592592592587E-2</v>
-      </c>
-      <c r="G5" s="1">
+        <v>5.000000000000001E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <f>Table1[[#This Row],[speed4]]*Table2[idle]/Table2[rated]</f>
+        <v>0.39090909090909104</v>
+      </c>
+      <c r="I5" s="1">
         <f>Table2[rated]/(Table1[[#This Row],[speed1]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>6031.8578948924032</v>
-      </c>
-      <c r="H5" s="1">
-        <f>Table2[rated]/(Table1[[#This Row],[speed2]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>3257.2032632418982</v>
-      </c>
-      <c r="I5" t="str">
-        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt; ",A2," km/h @ ",F2," rpm")</f>
-        <v xml:space="preserve">        &lt;efficiency ratio="0.005208" factor="0.7"/&gt; 0.05 km/h @ 800 rpm</v>
+        <v>6785.8401317539528</v>
+      </c>
+      <c r="J5" s="1">
+        <f>Table2[rated]/(Table1[[#This Row],[speed4]]/3.6 * 60 / (1*2*PI()))</f>
+        <v>867.95629592201703</v>
+      </c>
+      <c r="K5" t="str">
+        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt; &lt;!-- ",ROUND(Table1[[#This Row],[idleSpeed1]],2)," .. ",ROUND(Table1[[#This Row],[speed4]],1)," --&gt;")</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="0.020202" factor="0.6"/&gt; &lt;!-- 0.05 .. 0.9 --&gt;</v>
+      </c>
+      <c r="L5" t="str">
+        <f>Table1[[#This Row],[xml]]</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="0.020202" factor="0.6"/&gt; &lt;!-- 0.05 .. 0.9 --&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>1-Table2[range]</f>
-        <v>0.6</v>
+        <v>0.66666700000000001</v>
       </c>
       <c r="B6">
         <f>Table2[minEff]</f>
@@ -2135,37 +2250,49 @@
       </c>
       <c r="C6">
         <f>Table1[[#This Row],[ratio]]*Table2[s1]</f>
-        <v>16.2</v>
+        <v>3.6666685000000001</v>
       </c>
       <c r="D6">
+        <f>Table1[[#This Row],[ratio]]*Table2[s2]</f>
+        <v>7.3333370000000002</v>
+      </c>
+      <c r="E6">
+        <f>Table1[[#This Row],[ratio]]*Table2[s3]</f>
+        <v>14.666674</v>
+      </c>
+      <c r="F6">
         <f>Table1[[#This Row],[ratio]]*Table2[s4]</f>
-        <v>30</v>
-      </c>
-      <c r="E6" s="2">
+        <v>28.666681000000001</v>
+      </c>
+      <c r="G6" s="2">
         <f>Table1[[#This Row],[speed1]]*Table2[idle]/Table2[rated]</f>
-        <v>5.76</v>
-      </c>
-      <c r="F6" s="2">
-        <f>Table1[[#This Row],[speed2]]*Table2[idle]/Table2[rated]</f>
-        <v>10.666666666666666</v>
-      </c>
-      <c r="G6" s="1">
+        <v>1.650000825</v>
+      </c>
+      <c r="H6" s="2">
+        <f>Table1[[#This Row],[speed4]]*Table2[idle]/Table2[rated]</f>
+        <v>12.900006450000001</v>
+      </c>
+      <c r="I6" s="1">
         <f>Table2[rated]/(Table1[[#This Row],[speed1]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>52.359877559829883</v>
-      </c>
-      <c r="H6" s="1">
-        <f>Table2[rated]/(Table1[[#This Row],[speed2]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>28.274333882308138</v>
-      </c>
-      <c r="I6" t="str">
-        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt;")</f>
-        <v xml:space="preserve">        &lt;efficiency ratio="0.6" factor="0.88"/&gt;</v>
+        <v>205.63141632835104</v>
+      </c>
+      <c r="J6" s="1">
+        <f>Table2[rated]/(Table1[[#This Row],[speed4]]/3.6 * 60 / (1*2*PI()))</f>
+        <v>26.301692786184436</v>
+      </c>
+      <c r="K6" t="str">
+        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt; &lt;!-- ",ROUND(Table1[[#This Row],[idleSpeed1]],2)," .. ",ROUND(Table1[[#This Row],[speed4]],1)," --&gt;")</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="0.666667" factor="0.88"/&gt; &lt;!-- 1.65 .. 28.7 --&gt;</v>
+      </c>
+      <c r="L6" t="str">
+        <f>Table1[[#This Row],[xml]]</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="0.666667" factor="0.88"/&gt; &lt;!-- 1.65 .. 28.7 --&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>1-Table2[constF1]*Table2[range]</f>
-        <v>0.91999999999999993</v>
+        <v>0.90000009999999997</v>
       </c>
       <c r="B7">
         <f>Table2[minEff]+Table2[constF2]*(Table2[maxEff]-Table2[minEff])</f>
@@ -2173,31 +2300,43 @@
       </c>
       <c r="C7">
         <f>Table1[[#This Row],[ratio]]*Table2[s1]</f>
-        <v>24.839999999999996</v>
+        <v>4.9500005499999995</v>
       </c>
       <c r="D7">
+        <f>Table1[[#This Row],[ratio]]*Table2[s2]</f>
+        <v>9.900001099999999</v>
+      </c>
+      <c r="E7">
+        <f>Table1[[#This Row],[ratio]]*Table2[s3]</f>
+        <v>19.800002199999998</v>
+      </c>
+      <c r="F7">
         <f>Table1[[#This Row],[ratio]]*Table2[s4]</f>
-        <v>46</v>
-      </c>
-      <c r="E7" s="2">
+        <v>38.700004299999996</v>
+      </c>
+      <c r="G7" s="2">
         <f>Table1[[#This Row],[speed1]]*Table2[idle]/Table2[rated]</f>
-        <v>8.831999999999999</v>
-      </c>
-      <c r="F7" s="2">
-        <f>Table1[[#This Row],[speed2]]*Table2[idle]/Table2[rated]</f>
-        <v>16.355555555555554</v>
-      </c>
-      <c r="G7" s="1">
+        <v>2.2275002474999996</v>
+      </c>
+      <c r="H7" s="2">
+        <f>Table1[[#This Row],[speed4]]*Table2[idle]/Table2[rated]</f>
+        <v>17.415001934999996</v>
+      </c>
+      <c r="I7" s="1">
         <f>Table2[rated]/(Table1[[#This Row],[speed1]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>34.147746234671672</v>
-      </c>
-      <c r="H7" s="1">
-        <f>Table2[rated]/(Table1[[#This Row],[speed2]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>18.439782966722699</v>
-      </c>
-      <c r="I7" t="str">
-        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt;")</f>
-        <v xml:space="preserve">        &lt;efficiency ratio="0.92" factor="0.96"/&gt;</v>
+        <v>152.31962688601124</v>
+      </c>
+      <c r="J7" s="1">
+        <f>Table2[rated]/(Table1[[#This Row],[speed4]]/3.6 * 60 / (1*2*PI()))</f>
+        <v>19.482742973792135</v>
+      </c>
+      <c r="K7" t="str">
+        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt; &lt;!-- ",ROUND(Table1[[#This Row],[idleSpeed1]],2)," .. ",ROUND(Table1[[#This Row],[speed4]],1)," --&gt;")</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="0.9" factor="0.96"/&gt; &lt;!-- 2.23 .. 38.7 --&gt;</v>
+      </c>
+      <c r="L7" t="str">
+        <f>Table1[[#This Row],[xml]]</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="0.9" factor="0.96"/&gt; &lt;!-- 2.23 .. 38.7 --&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2210,37 +2349,49 @@
       </c>
       <c r="C8" s="5">
         <f>Table1[[#This Row],[ratio]]*Table2[s1]</f>
-        <v>27</v>
+        <v>5.5</v>
       </c>
       <c r="D8" s="5">
+        <f>Table1[[#This Row],[ratio]]*Table2[s2]</f>
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <f>Table1[[#This Row],[ratio]]*Table2[s3]</f>
+        <v>22</v>
+      </c>
+      <c r="F8" s="5">
         <f>Table1[[#This Row],[ratio]]*Table2[s4]</f>
-        <v>50</v>
-      </c>
-      <c r="E8" s="2">
+        <v>43</v>
+      </c>
+      <c r="G8" s="2">
         <f>Table1[[#This Row],[speed1]]*Table2[idle]/Table2[rated]</f>
-        <v>9.6</v>
-      </c>
-      <c r="F8" s="2">
-        <f>Table1[[#This Row],[speed2]]*Table2[idle]/Table2[rated]</f>
-        <v>17.777777777777779</v>
-      </c>
-      <c r="G8" s="1">
+        <v>2.4750000000000001</v>
+      </c>
+      <c r="H8" s="2">
+        <f>Table1[[#This Row],[speed4]]*Table2[idle]/Table2[rated]</f>
+        <v>19.350000000000001</v>
+      </c>
+      <c r="I8" s="1">
         <f>Table2[rated]/(Table1[[#This Row],[speed1]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>31.415926535897931</v>
-      </c>
-      <c r="H8" s="1">
-        <f>Table2[rated]/(Table1[[#This Row],[speed2]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>16.964600329384883</v>
-      </c>
-      <c r="I8" s="5" t="str">
-        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt;")</f>
-        <v xml:space="preserve">        &lt;efficiency ratio="1" factor="0.98"/&gt;</v>
+        <v>137.0876794293728</v>
+      </c>
+      <c r="J8" s="1">
+        <f>Table2[rated]/(Table1[[#This Row],[speed4]]/3.6 * 60 / (1*2*PI()))</f>
+        <v>17.53447062468722</v>
+      </c>
+      <c r="K8" t="str">
+        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt; &lt;!-- ",ROUND(Table1[[#This Row],[idleSpeed1]],2)," .. ",ROUND(Table1[[#This Row],[speed4]],1)," --&gt;")</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="1" factor="0.98"/&gt; &lt;!-- 2.48 .. 43 --&gt;</v>
+      </c>
+      <c r="L8" t="str">
+        <f>Table1[[#This Row],[xml]]</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="1" factor="0.98"/&gt; &lt;!-- 2.48 .. 43 --&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>1+Table2[constF1]*Table2[range]</f>
-        <v>1.08</v>
+        <v>1.0999999</v>
       </c>
       <c r="B9">
         <f>Table2[minEff]+Table2[constF2]*(Table2[maxEff]-Table2[minEff])</f>
@@ -2248,37 +2399,49 @@
       </c>
       <c r="C9">
         <f>Table1[[#This Row],[ratio]]*Table2[s1]</f>
-        <v>29.160000000000004</v>
+        <v>6.0499994500000005</v>
       </c>
       <c r="D9">
+        <f>Table1[[#This Row],[ratio]]*Table2[s2]</f>
+        <v>12.099998900000001</v>
+      </c>
+      <c r="E9">
+        <f>Table1[[#This Row],[ratio]]*Table2[s3]</f>
+        <v>24.199997800000002</v>
+      </c>
+      <c r="F9">
         <f>Table1[[#This Row],[ratio]]*Table2[s4]</f>
-        <v>54</v>
-      </c>
-      <c r="E9" s="2">
+        <v>47.299995700000004</v>
+      </c>
+      <c r="G9" s="2">
         <f>Table1[[#This Row],[speed1]]*Table2[idle]/Table2[rated]</f>
-        <v>10.368000000000002</v>
-      </c>
-      <c r="F9" s="2">
-        <f>Table1[[#This Row],[speed2]]*Table2[idle]/Table2[rated]</f>
-        <v>19.2</v>
-      </c>
-      <c r="G9" s="1">
+        <v>2.7224997525000005</v>
+      </c>
+      <c r="H9" s="2">
+        <f>Table1[[#This Row],[speed4]]*Table2[idle]/Table2[rated]</f>
+        <v>21.284998065000003</v>
+      </c>
+      <c r="I9" s="1">
         <f>Table2[rated]/(Table1[[#This Row],[speed1]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>29.088820866572153</v>
-      </c>
-      <c r="H9" s="1">
-        <f>Table2[rated]/(Table1[[#This Row],[speed2]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>15.707963267948966</v>
-      </c>
-      <c r="I9" t="str">
-        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt;")</f>
-        <v xml:space="preserve">        &lt;efficiency ratio="1.08" factor="0.96"/&gt;</v>
+        <v>124.62517444717294</v>
+      </c>
+      <c r="J9" s="1">
+        <f>Table2[rated]/(Table1[[#This Row],[speed4]]/3.6 * 60 / (1*2*PI()))</f>
+        <v>15.940429289754677</v>
+      </c>
+      <c r="K9" t="str">
+        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt; &lt;!-- ",ROUND(Table1[[#This Row],[idleSpeed1]],2)," .. ",ROUND(Table1[[#This Row],[speed4]],1)," --&gt;")</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="1.1" factor="0.96"/&gt; &lt;!-- 2.72 .. 47.3 --&gt;</v>
+      </c>
+      <c r="L9" t="str">
+        <f>Table1[[#This Row],[xml]]</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="1.1" factor="0.96"/&gt; &lt;!-- 2.72 .. 47.3 --&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>1+Table2[range]</f>
-        <v>1.4</v>
+        <v>1.3333330000000001</v>
       </c>
       <c r="B10">
         <f>Table2[minEff]</f>
@@ -2286,39 +2449,225 @@
       </c>
       <c r="C10">
         <f>Table1[[#This Row],[ratio]]*Table2[s1]</f>
-        <v>37.799999999999997</v>
+        <v>7.3333315000000008</v>
       </c>
       <c r="D10">
+        <f>Table1[[#This Row],[ratio]]*Table2[s2]</f>
+        <v>14.666663000000002</v>
+      </c>
+      <c r="E10">
+        <f>Table1[[#This Row],[ratio]]*Table2[s3]</f>
+        <v>29.333326000000003</v>
+      </c>
+      <c r="F10">
         <f>Table1[[#This Row],[ratio]]*Table2[s4]</f>
-        <v>70</v>
-      </c>
-      <c r="E10" s="2">
+        <v>57.333319000000003</v>
+      </c>
+      <c r="G10" s="2">
         <f>Table1[[#This Row],[speed1]]*Table2[idle]/Table2[rated]</f>
-        <v>13.439999999999998</v>
-      </c>
-      <c r="F10" s="2">
-        <f>Table1[[#This Row],[speed2]]*Table2[idle]/Table2[rated]</f>
-        <v>24.888888888888889</v>
-      </c>
-      <c r="G10" s="1">
+        <v>3.2999991750000004</v>
+      </c>
+      <c r="H10" s="2">
+        <f>Table1[[#This Row],[speed4]]*Table2[idle]/Table2[rated]</f>
+        <v>25.799993550000003</v>
+      </c>
+      <c r="I10" s="1">
         <f>Table2[rated]/(Table1[[#This Row],[speed1]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>22.439947525641383</v>
-      </c>
-      <c r="H10" s="1">
-        <f>Table2[rated]/(Table1[[#This Row],[speed2]]/3.6 * 60 / (1*2*PI()))</f>
-        <v>12.117571663846347</v>
-      </c>
-      <c r="I10" t="str">
-        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt;")</f>
-        <v xml:space="preserve">        &lt;efficiency ratio="1.4" factor="0.88"/&gt;</v>
+        <v>102.8157852759759</v>
+      </c>
+      <c r="J10" s="1">
+        <f>Table2[rated]/(Table1[[#This Row],[speed4]]/3.6 * 60 / (1*2*PI()))</f>
+        <v>13.150856256229476</v>
+      </c>
+      <c r="K10" t="str">
+        <f>CONCATENATE("        &lt;efficiency ratio=""",ROUND(Table1[[#This Row],[ratio]],6),""" factor=""",ROUND(Table1[[#This Row],[factor]],3),"""/&gt; &lt;!-- ",ROUND(Table1[[#This Row],[idleSpeed1]],2)," .. ",ROUND(Table1[[#This Row],[speed4]],1)," --&gt;")</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="1.333333" factor="0.88"/&gt; &lt;!-- 3.3 .. 57.3 --&gt;</v>
+      </c>
+      <c r="L10" t="str">
+        <f>Table1[[#This Row],[xml]]</f>
+        <v xml:space="preserve">        &lt;efficiency ratio="1.333333" factor="0.88"/&gt; &lt;!-- 3.3 .. 57.3 --&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f>INDEX(Table2[],1,Table3[[#This Row],[gear]]+1)</f>
+        <v>5.5</v>
+      </c>
+      <c r="G13">
+        <f>$A$5*Table3[[#This Row],[speed]]*Table2[idle]/Table2[rated]</f>
+        <v>5.000000000000001E-2</v>
+      </c>
+      <c r="H13">
+        <f>$A$6*Table3[[#This Row],[speed]]*Table2[idle]/Table2[rated]</f>
+        <v>1.650000825</v>
+      </c>
+      <c r="I13">
+        <f>$A$6*Table3[[#This Row],[speed]]</f>
+        <v>3.6666685000000001</v>
+      </c>
+      <c r="J13">
+        <f>$A$10*Table3[[#This Row],[speed]]</f>
+        <v>7.3333315000000008</v>
+      </c>
+      <c r="K13" t="str">
+        <f>CONCATENATE("        &lt;gear speed=""",ROUND(Table3[[#This Row],[speed]],2),""" name=""""/&gt; &lt;!-- ",ROUND(Table3[[#This Row],[minSpeed]],2)," ",ROUND(Table3[[#This Row],[idleSpeed]],2)," ",ROUND(Table3[[#This Row],[fromSpeed]],0)," ",ROUND(Table3[[#This Row],[toSpeed]],0),"--&gt;")</f>
+        <v xml:space="preserve">        &lt;gear speed="5.5" name=""/&gt; &lt;!-- 0.05 1.65 4 7--&gt;</v>
+      </c>
+      <c r="L13" s="5" t="str">
+        <f>Table3[[#This Row],[xml]]</f>
+        <v xml:space="preserve">        &lt;gear speed="5.5" name=""/&gt; &lt;!-- 0.05 1.65 4 7--&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <f>INDEX(Table2[],1,Table3[[#This Row],[gear]]+1)</f>
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <f>$A$5*Table3[[#This Row],[speed]]*Table2[idle]/Table2[rated]</f>
+        <v>0.10000000000000002</v>
+      </c>
+      <c r="H14">
+        <f>$A$6*Table3[[#This Row],[speed]]*Table2[idle]/Table2[rated]</f>
+        <v>3.30000165</v>
+      </c>
+      <c r="I14">
+        <f>$A$6*Table3[[#This Row],[speed]]</f>
+        <v>7.3333370000000002</v>
+      </c>
+      <c r="J14">
+        <f>$A$10*Table3[[#This Row],[speed]]</f>
+        <v>14.666663000000002</v>
+      </c>
+      <c r="K14" t="str">
+        <f>CONCATENATE("        &lt;gear speed=""",ROUND(Table3[[#This Row],[speed]],2),""" name=""""/&gt; &lt;!-- ",ROUND(Table3[[#This Row],[minSpeed]],2)," ",ROUND(Table3[[#This Row],[idleSpeed]],2)," ",ROUND(Table3[[#This Row],[fromSpeed]],0)," ",ROUND(Table3[[#This Row],[toSpeed]],0),"--&gt;")</f>
+        <v xml:space="preserve">        &lt;gear speed="11" name=""/&gt; &lt;!-- 0.1 3.3 7 15--&gt;</v>
+      </c>
+      <c r="L14" s="5" t="str">
+        <f>Table3[[#This Row],[xml]]</f>
+        <v xml:space="preserve">        &lt;gear speed="11" name=""/&gt; &lt;!-- 0.1 3.3 7 15--&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <f>INDEX(Table2[],1,Table3[[#This Row],[gear]]+1)</f>
+        <v>22</v>
+      </c>
+      <c r="G15">
+        <f>$A$5*Table3[[#This Row],[speed]]*Table2[idle]/Table2[rated]</f>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="H15">
+        <f>$A$6*Table3[[#This Row],[speed]]*Table2[idle]/Table2[rated]</f>
+        <v>6.6000033</v>
+      </c>
+      <c r="I15">
+        <f>$A$6*Table3[[#This Row],[speed]]</f>
+        <v>14.666674</v>
+      </c>
+      <c r="J15">
+        <f>$A$10*Table3[[#This Row],[speed]]</f>
+        <v>29.333326000000003</v>
+      </c>
+      <c r="K15" t="str">
+        <f>CONCATENATE("        &lt;gear speed=""",ROUND(Table3[[#This Row],[speed]],2),""" name=""""/&gt; &lt;!-- ",ROUND(Table3[[#This Row],[minSpeed]],2)," ",ROUND(Table3[[#This Row],[idleSpeed]],2)," ",ROUND(Table3[[#This Row],[fromSpeed]],0)," ",ROUND(Table3[[#This Row],[toSpeed]],0),"--&gt;")</f>
+        <v xml:space="preserve">        &lt;gear speed="22" name=""/&gt; &lt;!-- 0.2 6.6 15 29--&gt;</v>
+      </c>
+      <c r="L15" s="5" t="str">
+        <f>Table3[[#This Row],[xml]]</f>
+        <v xml:space="preserve">        &lt;gear speed="22" name=""/&gt; &lt;!-- 0.2 6.6 15 29--&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <f>INDEX(Table2[],1,Table3[[#This Row],[gear]]+1)</f>
+        <v>43</v>
+      </c>
+      <c r="G16">
+        <f>$A$5*Table3[[#This Row],[speed]]*Table2[idle]/Table2[rated]</f>
+        <v>0.39090909090909104</v>
+      </c>
+      <c r="H16">
+        <f>$A$6*Table3[[#This Row],[speed]]*Table2[idle]/Table2[rated]</f>
+        <v>12.900006450000001</v>
+      </c>
+      <c r="I16">
+        <f>$A$6*Table3[[#This Row],[speed]]</f>
+        <v>28.666681000000001</v>
+      </c>
+      <c r="J16">
+        <f>$A$10*Table3[[#This Row],[speed]]</f>
+        <v>57.333319000000003</v>
+      </c>
+      <c r="K16" t="str">
+        <f>CONCATENATE("        &lt;gear speed=""",ROUND(Table3[[#This Row],[speed]],2),""" name=""""/&gt; &lt;!-- ",ROUND(Table3[[#This Row],[minSpeed]],2)," ",ROUND(Table3[[#This Row],[idleSpeed]],2)," ",ROUND(Table3[[#This Row],[fromSpeed]],0)," ",ROUND(Table3[[#This Row],[toSpeed]],0),"--&gt;")</f>
+        <v xml:space="preserve">        &lt;gear speed="43" name=""/&gt; &lt;!-- 0.39 12.9 29 57--&gt;</v>
+      </c>
+      <c r="L16" s="5" t="str">
+        <f>Table3[[#This Row],[xml]]</f>
+        <v xml:space="preserve">        &lt;gear speed="43" name=""/&gt; &lt;!-- 0.39 12.9 29 57--&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>